<commit_message>
email sending ability added
</commit_message>
<xml_diff>
--- a/src/excelSender/sourceTable/Table.xlsx
+++ b/src/excelSender/sourceTable/Table.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>ФИО</t>
   </si>
@@ -39,7 +39,19 @@
     <t>Гадельшин Ильдар Фанисович</t>
   </si>
   <si>
-    <t>warrior@gmail.com</t>
+    <t>Письмо отправлено</t>
+  </si>
+  <si>
+    <t>Нет</t>
+  </si>
+  <si>
+    <t>Гадельшин Ильша Фанисович</t>
+  </si>
+  <si>
+    <t>Иванов Иван Иванович</t>
+  </si>
+  <si>
+    <t>ilshat.koyash@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -93,7 +105,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -106,6 +118,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -388,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -396,12 +411,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -411,75 +427,120 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3">
-        <v>45526</v>
+        <v>45532</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3">
-        <v>45435</v>
+        <v>45532</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3">
+        <v>45532</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3">
+        <v>45532</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>45532</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3">
+        <v>45532</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -487,9 +548,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C3:C7" r:id="rId2" display="vinnie8warrior@gmail.com"/>
+    <hyperlink ref="C7" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>